<commit_message>
EI Variable Installments T2 scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2389-MS-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-WaiveInterest-DLR-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/2389-MS-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-WaiveInterest-DLR-Newcreateloan1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -664,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1657,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
-        <v>9</v>
+        <v>1363</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>27</v>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="11">
-        <v>0</v>
+        <v>33.97</v>
       </c>
       <c r="H2" s="11">
         <v>0</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
-        <v>7</v>
+        <v>1350</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>27</v>

</xml_diff>